<commit_message>
mt seqs and concs
</commit_message>
<xml_diff>
--- a/Frogs/Lab/Seq_test.xlsx
+++ b/Frogs/Lab/Seq_test.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danieljeffries/Dropbox/TPing/2019/MolGen_2019/Frogs/Lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danieljeffries/Dropbox/TPing/2019/MolGen_2019/MolGen_2019_students/Frogs/Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E18978F-29EC-0645-9CB8-9E8AFBF9F4FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3AF5E6-4D5E-0642-A0A4-48344F9F6B8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{421A9A2D-B5A5-3942-9891-B20BD0D2EDC4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{421A9A2D-B5A5-3942-9891-B20BD0D2EDC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="206">
   <si>
     <t>Pop</t>
   </si>
@@ -215,13 +217,448 @@
   </si>
   <si>
     <t>rag1 R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alignment </t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>F ab1</t>
+  </si>
+  <si>
+    <t>R ab1</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>ok/bad</t>
+  </si>
+  <si>
+    <t>good/ok</t>
+  </si>
+  <si>
+    <t>pop code</t>
+  </si>
+  <si>
+    <t>Ellouène</t>
+  </si>
+  <si>
+    <t>Charavel</t>
+  </si>
+  <si>
+    <t>&lt;ellouene.charavel@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Vivien</t>
+  </si>
+  <si>
+    <t>Cosandey</t>
+  </si>
+  <si>
+    <t>&lt;vivien.cosandey@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Hulaas</t>
+  </si>
+  <si>
+    <t>&lt;lisa.hulaas@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Nora</t>
+  </si>
+  <si>
+    <t>Khelidj</t>
+  </si>
+  <si>
+    <t>&lt;nora.khelidj@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Silvana</t>
+  </si>
+  <si>
+    <t>Manzocchi</t>
+  </si>
+  <si>
+    <t>&lt;silvana.manzocchi@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Mattatia</t>
+  </si>
+  <si>
+    <t>&lt;ivan.mattatia@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Angie</t>
+  </si>
+  <si>
+    <t>&lt;angie.orejuelayustes@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>Rausa</t>
+  </si>
+  <si>
+    <t>&lt;nicolas.rausa@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Aurélien</t>
+  </si>
+  <si>
+    <t>Rochat</t>
+  </si>
+  <si>
+    <t>&lt;aurelien.rochat@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>Royston</t>
+  </si>
+  <si>
+    <t>&lt;arthur.royston@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Ludovic</t>
+  </si>
+  <si>
+    <t>Rüedi</t>
+  </si>
+  <si>
+    <t>&lt;ludovic.ruedi@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Angela</t>
+  </si>
+  <si>
+    <t>&lt;angela.ruizdepaz@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>&lt;heather_2108@hotmail.com&gt;,</t>
+  </si>
+  <si>
+    <t>Zoé</t>
+  </si>
+  <si>
+    <t>Siegel</t>
+  </si>
+  <si>
+    <t>&lt;zoe.siegel@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Benoit</t>
+  </si>
+  <si>
+    <t>Sommervogel</t>
+  </si>
+  <si>
+    <t>&lt;benoit.sommervogel@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Wildi</t>
+  </si>
+  <si>
+    <t>&lt;julia.wildi@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Zermatten</t>
+  </si>
+  <si>
+    <t>&lt;lucas.zermatten@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>&lt;Sarah.Descloux@unifr.ch&gt;,</t>
+  </si>
+  <si>
+    <t>&lt;Noemie.ioset@unifr.ch&gt;,</t>
+  </si>
+  <si>
+    <t>&lt;vincent.grognuz@unifr.ch&gt;,</t>
+  </si>
+  <si>
+    <t>&lt;annie.guillaume@epfl.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Roxane</t>
+  </si>
+  <si>
+    <t>Allemann</t>
+  </si>
+  <si>
+    <t>&lt;roxane.allemann@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Bergerat</t>
+  </si>
+  <si>
+    <t>&lt;charlotte.bergerat@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>Dany</t>
+  </si>
+  <si>
+    <t>Buffat</t>
+  </si>
+  <si>
+    <t>&lt;dany.buffat@unil.ch&gt;,</t>
+  </si>
+  <si>
+    <t>&lt;morgane.calvani@yahoo.fr&gt;</t>
+  </si>
+  <si>
+    <t>Orejuela Yustes</t>
+  </si>
+  <si>
+    <t>Ruiz De Paz</t>
+  </si>
+  <si>
+    <t>1_PIA_07_cytb</t>
+  </si>
+  <si>
+    <t>1_PIA_14_cytb</t>
+  </si>
+  <si>
+    <t>2_CRE_05_cytb</t>
+  </si>
+  <si>
+    <t>2_CRE_11_cytb</t>
+  </si>
+  <si>
+    <t>3_SGI_05_cytb</t>
+  </si>
+  <si>
+    <t>3_SGI_08_cytb</t>
+  </si>
+  <si>
+    <t>3_SGI_09_cytb</t>
+  </si>
+  <si>
+    <t>3_SGI_11_cytb</t>
+  </si>
+  <si>
+    <t>4_ALB_03_cytb</t>
+  </si>
+  <si>
+    <t>4_ALB_09_cytb</t>
+  </si>
+  <si>
+    <t>5_PUA_03_cytb</t>
+  </si>
+  <si>
+    <t>5_PUA_07_cytb</t>
+  </si>
+  <si>
+    <t>6_LDC_03_cytb</t>
+  </si>
+  <si>
+    <t>6_LDC_04_cytb</t>
+  </si>
+  <si>
+    <t>6_LDC_06_cytb</t>
+  </si>
+  <si>
+    <t>6_LDC_11_cytb</t>
+  </si>
+  <si>
+    <t>6_LDC_16_cytb</t>
+  </si>
+  <si>
+    <t>7_LDS_03_cytb</t>
+  </si>
+  <si>
+    <t>7_LDS_07_cytb</t>
+  </si>
+  <si>
+    <t>8_MAG_04_cytb</t>
+  </si>
+  <si>
+    <t>8_MAG_05_cytb</t>
+  </si>
+  <si>
+    <t>8_MAG_10_cytb</t>
+  </si>
+  <si>
+    <t>9_BAG_07_cytb</t>
+  </si>
+  <si>
+    <t>9_BAG_09_cytb</t>
+  </si>
+  <si>
+    <t>9_BAG_17_cytb</t>
+  </si>
+  <si>
+    <t>10_SSE_02_cytb</t>
+  </si>
+  <si>
+    <t>10_SSE_04_Cytb</t>
+  </si>
+  <si>
+    <t>10_SSE_13_cytb</t>
+  </si>
+  <si>
+    <t>12_ROS_04_cytb</t>
+  </si>
+  <si>
+    <t>12_ROS_05_cytb</t>
+  </si>
+  <si>
+    <t>3_SGI_12_cytb F</t>
+  </si>
+  <si>
+    <t>calvani</t>
+  </si>
+  <si>
+    <t>Morgane</t>
+  </si>
+  <si>
+    <t>Descloux</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Noemie</t>
+  </si>
+  <si>
+    <t>Annie</t>
+  </si>
+  <si>
+    <t>Vincent</t>
+  </si>
+  <si>
+    <t>Ioset</t>
+  </si>
+  <si>
+    <t>Grognuz</t>
+  </si>
+  <si>
+    <t>Guillaume</t>
+  </si>
+  <si>
+    <t>1_PIA_09_cytb</t>
+  </si>
+  <si>
+    <t>1_PIA_11_cytb</t>
+  </si>
+  <si>
+    <t>2_CRE_08_cytb</t>
+  </si>
+  <si>
+    <t>2_CRE_12_cytb</t>
+  </si>
+  <si>
+    <t>3_SGI_02_cytb</t>
+  </si>
+  <si>
+    <t>3_SGI_03_cytb</t>
+  </si>
+  <si>
+    <t>3_SGI_04_cytb</t>
+  </si>
+  <si>
+    <t>3_SGI_14_cytb</t>
+  </si>
+  <si>
+    <t>3_SGI_16_cytb</t>
+  </si>
+  <si>
+    <t>4_ALB_06_cytb</t>
+  </si>
+  <si>
+    <t>4_ALB_07_cytb</t>
+  </si>
+  <si>
+    <t>5_PUA_02_cytb</t>
+  </si>
+  <si>
+    <t>5_PUA_09_cytb</t>
+  </si>
+  <si>
+    <t>6_LDC_05_cytb</t>
+  </si>
+  <si>
+    <t>6_LDC_08_cytb</t>
+  </si>
+  <si>
+    <t>6_LDC_10_cytb</t>
+  </si>
+  <si>
+    <t>6_LDC_13_cytb</t>
+  </si>
+  <si>
+    <t>6_LDC_15_cytb</t>
+  </si>
+  <si>
+    <t>7_LDS_01_cytb</t>
+  </si>
+  <si>
+    <t>7_LDS_10_cytb</t>
+  </si>
+  <si>
+    <t>8_MAG_02_cytb</t>
+  </si>
+  <si>
+    <t>8_MAG_09_cytb</t>
+  </si>
+  <si>
+    <t>8_MAG_11_cytb</t>
+  </si>
+  <si>
+    <t>9_BAG_02_cytb</t>
+  </si>
+  <si>
+    <t>9_BAG_03_cytb</t>
+  </si>
+  <si>
+    <t>9_BAG_12_cytb</t>
+  </si>
+  <si>
+    <t>10_SSE_03_cytb</t>
+  </si>
+  <si>
+    <t>10_SSE_05_Cytb</t>
+  </si>
+  <si>
+    <t>10_SSE_10_cytb</t>
+  </si>
+  <si>
+    <t>12_ROS_07_cytb</t>
+  </si>
+  <si>
+    <t>12_ROS_09_cytb</t>
+  </si>
+  <si>
+    <t>Heather</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,6 +685,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -361,7 +804,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -370,9 +813,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -380,17 +820,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803D3B72-74BB-024E-90BB-1E95E82F18E1}">
   <dimension ref="A2:R48"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,20 +1161,20 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="12" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="13"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="H3" s="8"/>
-      <c r="I3" s="10" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11" t="s">
+      <c r="J3" s="9"/>
+      <c r="K3" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -744,44 +1188,44 @@
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>2.5</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="14">
+      <c r="J4" s="4"/>
+      <c r="K4" s="11">
         <f>SUM(I4)*27</f>
         <v>67.5</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="12">
         <v>95</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>0.5</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="14">
+      <c r="J5" s="4"/>
+      <c r="K5" s="11">
         <f t="shared" ref="K5:K10" si="0">SUM(I5)*27</f>
         <v>13.5</v>
       </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15">
+      <c r="M5" s="12"/>
+      <c r="N5" s="12">
         <v>95</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="12" t="s">
         <v>54</v>
       </c>
     </row>
@@ -795,22 +1239,22 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>1.25</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="14">
+      <c r="J6" s="4"/>
+      <c r="K6" s="11">
         <f t="shared" si="0"/>
         <v>33.75</v>
       </c>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15">
+      <c r="M6" s="12"/>
+      <c r="N6" s="12">
         <v>56</v>
       </c>
-      <c r="O6" s="15">
+      <c r="O6" s="12">
         <v>1</v>
       </c>
     </row>
@@ -824,22 +1268,22 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>1.25</v>
       </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="14">
+      <c r="J7" s="4"/>
+      <c r="K7" s="11">
         <f t="shared" si="0"/>
         <v>33.75</v>
       </c>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15">
+      <c r="M7" s="12"/>
+      <c r="N7" s="12">
         <v>72</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="12">
         <v>1</v>
       </c>
     </row>
@@ -853,22 +1297,22 @@
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>1</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="14">
+      <c r="J8" s="4"/>
+      <c r="K8" s="11">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15">
+      <c r="M8" s="12"/>
+      <c r="N8" s="12">
         <v>72</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="12">
         <v>10</v>
       </c>
     </row>
@@ -882,14 +1326,14 @@
       <c r="D9">
         <v>2</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>0.1</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="8">
+      <c r="J9" s="4"/>
+      <c r="K9" s="7">
         <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
@@ -904,15 +1348,15 @@
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <f>25-SUM(I4:I9)</f>
         <v>18.399999999999999</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="14">
+      <c r="J10" s="4"/>
+      <c r="K10" s="11">
         <f t="shared" si="0"/>
         <v>496.79999999999995</v>
       </c>
@@ -927,10 +1371,10 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="8"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="3">
@@ -942,13 +1386,13 @@
       <c r="D12">
         <v>2</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="6">
+      <c r="H12" s="8"/>
+      <c r="I12" s="5">
         <f>SUM(I4:I11)</f>
         <v>25</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="9">
+      <c r="J12" s="5"/>
+      <c r="K12" s="8">
         <f>SUM(K4:K10)</f>
         <v>675</v>
       </c>
@@ -1007,12 +1451,12 @@
       <c r="D17">
         <v>2</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="12" t="s">
+      <c r="H17" s="6"/>
+      <c r="I17" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="13"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
@@ -1024,47 +1468,47 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="10" t="s">
+      <c r="H18" s="7"/>
+      <c r="I18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="11" t="s">
+      <c r="J18" s="9"/>
+      <c r="K18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M18" s="15" t="s">
+      <c r="M18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="N18" s="15">
+      <c r="N18" s="12">
         <v>95</v>
       </c>
-      <c r="O18" s="15" t="s">
+      <c r="O18" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="R18" s="16">
+      <c r="R18" s="13">
         <v>18.399999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="4">
         <v>2.5</v>
       </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="14">
+      <c r="J19" s="4"/>
+      <c r="K19" s="11">
         <f>SUM(I19)*27</f>
         <v>67.5</v>
       </c>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15">
+      <c r="M19" s="12"/>
+      <c r="N19" s="12">
         <v>95</v>
       </c>
-      <c r="O19" s="15" t="s">
+      <c r="O19" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="R19" s="16">
+      <c r="R19" s="13">
         <v>2.5</v>
       </c>
     </row>
@@ -1081,113 +1525,113 @@
         <f>SUM(C20:D20)</f>
         <v>48</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="4">
         <v>0.47499999999999998</v>
       </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="14">
+      <c r="J20" s="4"/>
+      <c r="K20" s="11">
         <f t="shared" ref="K20:K25" si="1">SUM(I20)*27</f>
         <v>12.824999999999999</v>
       </c>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15">
+      <c r="M20" s="12"/>
+      <c r="N20" s="12">
         <v>56</v>
       </c>
-      <c r="O20" s="15">
+      <c r="O20" s="12">
         <v>1</v>
       </c>
-      <c r="R20" s="16">
+      <c r="R20" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="4">
         <v>1.25</v>
       </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="14">
+      <c r="J21" s="4"/>
+      <c r="K21" s="11">
         <f t="shared" si="1"/>
         <v>33.75</v>
       </c>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15">
+      <c r="M21" s="12"/>
+      <c r="N21" s="12">
         <v>72</v>
       </c>
-      <c r="O21" s="15">
+      <c r="O21" s="12">
         <v>1</v>
       </c>
-      <c r="R21" s="16">
+      <c r="R21" s="13">
         <v>1.25</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="4">
         <v>1.25</v>
       </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="14">
+      <c r="J22" s="4"/>
+      <c r="K22" s="11">
         <f t="shared" si="1"/>
         <v>33.75</v>
       </c>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15">
+      <c r="M22" s="12"/>
+      <c r="N22" s="12">
         <v>72</v>
       </c>
-      <c r="O22" s="15">
+      <c r="O22" s="12">
         <v>10</v>
       </c>
       <c r="P22">
         <v>1</v>
       </c>
-      <c r="R22" s="16">
+      <c r="R22" s="13">
         <v>1.25</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="4">
         <v>2</v>
       </c>
-      <c r="J23" s="5"/>
-      <c r="K23" s="14">
+      <c r="J23" s="4"/>
+      <c r="K23" s="11">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="R23" s="16">
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="R23" s="13">
         <v>0.1</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="H24" s="8" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="H24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="4">
         <v>0.125</v>
       </c>
-      <c r="J24" s="5"/>
-      <c r="K24" s="8">
+      <c r="J24" s="4"/>
+      <c r="K24" s="7">
         <f t="shared" si="1"/>
         <v>3.375</v>
       </c>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
       <c r="R24">
         <f>SUM(R18:R23)</f>
         <v>24</v>
@@ -1206,21 +1650,21 @@
       <c r="D25" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="4">
         <f>25-SUM(I19:I24)</f>
         <v>17.399999999999999</v>
       </c>
-      <c r="J25" s="5"/>
-      <c r="K25" s="14">
+      <c r="J25" s="4"/>
+      <c r="K25" s="11">
         <f t="shared" si="1"/>
         <v>469.79999999999995</v>
       </c>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1235,13 +1679,13 @@
       <c r="D26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="8"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="7"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1256,19 +1700,19 @@
       <c r="D27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="6">
+      <c r="H27" s="8"/>
+      <c r="I27" s="5">
         <f>SUM(I19:I25)</f>
         <v>25</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="9">
+      <c r="J27" s="5"/>
+      <c r="K27" s="8">
         <f>SUM(K19:K25)</f>
         <v>675</v>
       </c>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1506,10 +1950,618 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1D4683-9771-CD4B-9DAF-C7BFA0A5D23C}">
+  <dimension ref="A2:N28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="M11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="M13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14">
+        <v>6</v>
+      </c>
+      <c r="M14" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15">
+        <v>7</v>
+      </c>
+      <c r="M15" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17">
+        <v>17</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17">
+        <v>9</v>
+      </c>
+      <c r="M17" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>18</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" t="s">
+        <v>66</v>
+      </c>
+      <c r="K18">
+        <v>9</v>
+      </c>
+      <c r="M18" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19">
+        <v>23</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K19">
+        <v>12</v>
+      </c>
+      <c r="M19" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>24</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20">
+        <v>12</v>
+      </c>
+      <c r="M20" t="s">
+        <v>25</v>
+      </c>
+      <c r="N20" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F8C7D2-6725-DA4C-AC0D-D94EE0202768}">
   <dimension ref="B2:N98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P82" sqref="P82"/>
     </sheetView>
   </sheetViews>
@@ -1541,7 +2593,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:G9" si="0">B3&amp;C3&amp;D3</f>
+        <f t="shared" ref="E3:E9" si="0">B3&amp;C3&amp;D3</f>
         <v>2rag1F</v>
       </c>
       <c r="H3">
@@ -1759,7 +2811,7 @@
         <v>8</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" ref="E13:G19" si="1">B13&amp;C13&amp;D13</f>
+        <f t="shared" ref="E13:E19" si="1">B13&amp;C13&amp;D13</f>
         <v>2rag1R</v>
       </c>
     </row>
@@ -2506,4 +3558,498 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7B1BDD-6332-4941-A648-433A6B489CB7}">
+  <dimension ref="A4:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" t="s">
+        <v>176</v>
+      </c>
+      <c r="E21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>177</v>
+      </c>
+      <c r="E22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E23" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" t="s">
+        <v>179</v>
+      </c>
+      <c r="E24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" t="s">
+        <v>180</v>
+      </c>
+      <c r="E25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" t="s">
+        <v>181</v>
+      </c>
+      <c r="E26" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" t="s">
+        <v>182</v>
+      </c>
+      <c r="E27" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" t="s">
+        <v>183</v>
+      </c>
+      <c r="E28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>184</v>
+      </c>
+      <c r="E32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E33" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>186</v>
+      </c>
+      <c r="E34" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>190</v>
+      </c>
+      <c r="E36" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>191</v>
+      </c>
+      <c r="E37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>